<commit_message>
Use datetime and improve test data
</commit_message>
<xml_diff>
--- a/docs/source/_static/structure/IFDAT_DATAMODEL.xlsx
+++ b/docs/source/_static/structure/IFDAT_DATAMODEL.xlsx
@@ -10,7 +10,7 @@
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="COVER" sheetId="1" state="visible" r:id="rId1"/>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="DATA_STRUCTURE" sheetId="2" state="visible" r:id="rId2"/>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="ORG" sheetId="3" state="visible" r:id="rId3"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="DATE" sheetId="4" state="visible" r:id="rId4"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="DATETIME" sheetId="4" state="visible" r:id="rId4"/>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="STR" sheetId="5" state="visible" r:id="rId5"/>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="STR128" sheetId="6" state="visible" r:id="rId6"/>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="STR64" sheetId="7" state="visible" r:id="rId7"/>
@@ -6499,7 +6499,7 @@
       </c>
       <c r="D3" s="6" t="inlineStr">
         <is>
-          <t>DATE</t>
+          <t>DATETIME</t>
         </is>
       </c>
       <c r="E3" s="7" t="inlineStr">
@@ -6526,7 +6526,7 @@
       </c>
       <c r="D4" s="6" t="inlineStr">
         <is>
-          <t>DATE</t>
+          <t>DATETIME</t>
         </is>
       </c>
       <c r="E4" s="7" t="inlineStr">
@@ -6715,7 +6715,7 @@
       </c>
       <c r="D11" s="9" t="inlineStr">
         <is>
-          <t>DATE</t>
+          <t>DATETIME</t>
         </is>
       </c>
       <c r="E11" s="10" t="inlineStr">
@@ -6742,7 +6742,7 @@
       </c>
       <c r="D12" s="9" t="inlineStr">
         <is>
-          <t>DATE</t>
+          <t>DATETIME</t>
         </is>
       </c>
       <c r="E12" s="10" t="inlineStr">
@@ -7579,7 +7579,7 @@
       </c>
       <c r="D43" s="6" t="inlineStr">
         <is>
-          <t>DATE</t>
+          <t>DATETIME</t>
         </is>
       </c>
       <c r="E43" s="7" t="inlineStr">
@@ -7606,7 +7606,7 @@
       </c>
       <c r="D44" s="6" t="inlineStr">
         <is>
-          <t>DATE</t>
+          <t>DATETIME</t>
         </is>
       </c>
       <c r="E44" s="7" t="inlineStr">
@@ -7633,7 +7633,7 @@
       </c>
       <c r="D45" s="6" t="inlineStr">
         <is>
-          <t>DATE</t>
+          <t>DATETIME</t>
         </is>
       </c>
       <c r="E45" s="7" t="inlineStr">
@@ -7768,7 +7768,7 @@
       </c>
       <c r="D50" s="6" t="inlineStr">
         <is>
-          <t>DATE</t>
+          <t>DATETIME</t>
         </is>
       </c>
       <c r="E50" s="7" t="inlineStr">
@@ -8200,7 +8200,7 @@
       </c>
       <c r="D66" s="6" t="inlineStr">
         <is>
-          <t>DATE</t>
+          <t>DATETIME</t>
         </is>
       </c>
       <c r="E66" s="7" t="inlineStr">
@@ -8227,7 +8227,7 @@
       </c>
       <c r="D67" s="6" t="inlineStr">
         <is>
-          <t>DATE</t>
+          <t>DATETIME</t>
         </is>
       </c>
       <c r="E67" s="7" t="inlineStr">
@@ -8443,7 +8443,7 @@
       </c>
       <c r="D75" s="9" t="inlineStr">
         <is>
-          <t>DATE</t>
+          <t>DATETIME</t>
         </is>
       </c>
       <c r="E75" s="10" t="inlineStr">
@@ -8470,7 +8470,7 @@
       </c>
       <c r="D76" s="9" t="inlineStr">
         <is>
-          <t>DATE</t>
+          <t>DATETIME</t>
         </is>
       </c>
       <c r="E76" s="10" t="inlineStr">
@@ -8578,7 +8578,7 @@
       </c>
       <c r="D80" s="9" t="inlineStr">
         <is>
-          <t>DATE</t>
+          <t>DATETIME</t>
         </is>
       </c>
       <c r="E80" s="10" t="inlineStr">
@@ -8713,7 +8713,7 @@
       </c>
       <c r="D85" s="6" t="inlineStr">
         <is>
-          <t>DATE</t>
+          <t>DATETIME</t>
         </is>
       </c>
       <c r="E85" s="7" t="inlineStr">
@@ -8821,7 +8821,7 @@
       </c>
       <c r="D89" s="9" t="inlineStr">
         <is>
-          <t>DATE</t>
+          <t>DATETIME</t>
         </is>
       </c>
       <c r="E89" s="10" t="inlineStr">
@@ -8902,7 +8902,7 @@
       </c>
       <c r="D92" s="6" t="inlineStr">
         <is>
-          <t>DATE</t>
+          <t>DATETIME</t>
         </is>
       </c>
       <c r="E92" s="7" t="inlineStr">
@@ -8929,7 +8929,7 @@
       </c>
       <c r="D93" s="6" t="inlineStr">
         <is>
-          <t>DATE</t>
+          <t>DATETIME</t>
         </is>
       </c>
       <c r="E93" s="7" t="inlineStr">
@@ -9091,7 +9091,7 @@
       </c>
       <c r="D99" s="9" t="inlineStr">
         <is>
-          <t>DATE</t>
+          <t>DATETIME</t>
         </is>
       </c>
       <c r="E99" s="10" t="inlineStr">
@@ -9118,7 +9118,7 @@
       </c>
       <c r="D100" s="9" t="inlineStr">
         <is>
-          <t>DATE</t>
+          <t>DATETIME</t>
         </is>
       </c>
       <c r="E100" s="10" t="inlineStr">
@@ -9388,7 +9388,7 @@
       </c>
       <c r="D110" s="6" t="inlineStr">
         <is>
-          <t>DATE</t>
+          <t>DATETIME</t>
         </is>
       </c>
       <c r="E110" s="7" t="inlineStr">
@@ -9415,7 +9415,7 @@
       </c>
       <c r="D111" s="6" t="inlineStr">
         <is>
-          <t>DATE</t>
+          <t>DATETIME</t>
         </is>
       </c>
       <c r="E111" s="7" t="inlineStr">
@@ -9442,7 +9442,7 @@
       </c>
       <c r="D112" s="6" t="inlineStr">
         <is>
-          <t>DATE</t>
+          <t>DATETIME</t>
         </is>
       </c>
       <c r="E112" s="7" t="inlineStr">
@@ -9469,7 +9469,7 @@
       </c>
       <c r="D113" s="6" t="inlineStr">
         <is>
-          <t>DATE</t>
+          <t>DATETIME</t>
         </is>
       </c>
       <c r="E113" s="7" t="inlineStr">
@@ -9631,7 +9631,7 @@
       </c>
       <c r="D119" s="9" t="inlineStr">
         <is>
-          <t>DATE</t>
+          <t>DATETIME</t>
         </is>
       </c>
       <c r="E119" s="10" t="inlineStr">
@@ -9712,7 +9712,7 @@
       </c>
       <c r="D122" s="6" t="inlineStr">
         <is>
-          <t>DATE</t>
+          <t>DATETIME</t>
         </is>
       </c>
       <c r="E122" s="7" t="inlineStr">
@@ -9739,7 +9739,7 @@
       </c>
       <c r="D123" s="6" t="inlineStr">
         <is>
-          <t>DATE</t>
+          <t>DATETIME</t>
         </is>
       </c>
       <c r="E123" s="7" t="inlineStr">
@@ -9928,7 +9928,7 @@
       </c>
       <c r="D130" s="9" t="inlineStr">
         <is>
-          <t>DATE</t>
+          <t>DATETIME</t>
         </is>
       </c>
       <c r="E130" s="10" t="inlineStr">
@@ -9955,7 +9955,7 @@
       </c>
       <c r="D131" s="9" t="inlineStr">
         <is>
-          <t>DATE</t>
+          <t>DATETIME</t>
         </is>
       </c>
       <c r="E131" s="10" t="inlineStr">
@@ -10468,7 +10468,7 @@
       </c>
       <c r="D150" s="9" t="inlineStr">
         <is>
-          <t>DATE</t>
+          <t>DATETIME</t>
         </is>
       </c>
       <c r="E150" s="10" t="inlineStr">
@@ -10495,7 +10495,7 @@
       </c>
       <c r="D151" s="9" t="inlineStr">
         <is>
-          <t>DATE</t>
+          <t>DATETIME</t>
         </is>
       </c>
       <c r="E151" s="10" t="inlineStr">
@@ -10630,7 +10630,7 @@
       </c>
       <c r="D156" s="6" t="inlineStr">
         <is>
-          <t>DATE</t>
+          <t>DATETIME</t>
         </is>
       </c>
       <c r="E156" s="7" t="inlineStr">
@@ -10657,7 +10657,7 @@
       </c>
       <c r="D157" s="6" t="inlineStr">
         <is>
-          <t>DATE</t>
+          <t>DATETIME</t>
         </is>
       </c>
       <c r="E157" s="7" t="inlineStr">
@@ -10819,7 +10819,7 @@
       </c>
       <c r="D163" s="9" t="inlineStr">
         <is>
-          <t>DATE</t>
+          <t>DATETIME</t>
         </is>
       </c>
       <c r="E163" s="10" t="inlineStr">
@@ -10846,7 +10846,7 @@
       </c>
       <c r="D164" s="9" t="inlineStr">
         <is>
-          <t>DATE</t>
+          <t>DATETIME</t>
         </is>
       </c>
       <c r="E164" s="10" t="inlineStr">
@@ -11062,7 +11062,7 @@
       </c>
       <c r="D172" s="6" t="inlineStr">
         <is>
-          <t>DATE</t>
+          <t>DATETIME</t>
         </is>
       </c>
       <c r="E172" s="7" t="inlineStr">
@@ -11089,7 +11089,7 @@
       </c>
       <c r="D173" s="6" t="inlineStr">
         <is>
-          <t>DATE</t>
+          <t>DATETIME</t>
         </is>
       </c>
       <c r="E173" s="7" t="inlineStr">
@@ -11278,7 +11278,7 @@
       </c>
       <c r="D180" s="9" t="inlineStr">
         <is>
-          <t>DATE</t>
+          <t>DATETIME</t>
         </is>
       </c>
       <c r="E180" s="10" t="inlineStr">
@@ -11305,7 +11305,7 @@
       </c>
       <c r="D181" s="9" t="inlineStr">
         <is>
-          <t>DATE</t>
+          <t>DATETIME</t>
         </is>
       </c>
       <c r="E181" s="10" t="inlineStr">
@@ -11494,7 +11494,7 @@
       </c>
       <c r="D188" s="6" t="inlineStr">
         <is>
-          <t>DATE</t>
+          <t>DATETIME</t>
         </is>
       </c>
       <c r="E188" s="7" t="inlineStr">
@@ -11521,7 +11521,7 @@
       </c>
       <c r="D189" s="6" t="inlineStr">
         <is>
-          <t>DATE</t>
+          <t>DATETIME</t>
         </is>
       </c>
       <c r="E189" s="7" t="inlineStr">
@@ -11683,7 +11683,7 @@
       </c>
       <c r="D195" s="9" t="inlineStr">
         <is>
-          <t>DATE</t>
+          <t>DATETIME</t>
         </is>
       </c>
       <c r="E195" s="10" t="inlineStr">
@@ -11710,7 +11710,7 @@
       </c>
       <c r="D196" s="9" t="inlineStr">
         <is>
-          <t>DATE</t>
+          <t>DATETIME</t>
         </is>
       </c>
       <c r="E196" s="10" t="inlineStr">
@@ -11872,7 +11872,7 @@
       </c>
       <c r="D202" s="6" t="inlineStr">
         <is>
-          <t>DATE</t>
+          <t>DATETIME</t>
         </is>
       </c>
       <c r="E202" s="7" t="inlineStr">
@@ -11899,7 +11899,7 @@
       </c>
       <c r="D203" s="6" t="inlineStr">
         <is>
-          <t>DATE</t>
+          <t>DATETIME</t>
         </is>
       </c>
       <c r="E203" s="7" t="inlineStr">
@@ -12142,7 +12142,7 @@
       </c>
       <c r="D212" s="9" t="inlineStr">
         <is>
-          <t>DATE</t>
+          <t>DATETIME</t>
         </is>
       </c>
       <c r="E212" s="10" t="inlineStr">
@@ -12169,7 +12169,7 @@
       </c>
       <c r="D213" s="9" t="inlineStr">
         <is>
-          <t>DATE</t>
+          <t>DATETIME</t>
         </is>
       </c>
       <c r="E213" s="10" t="inlineStr">
@@ -12412,7 +12412,7 @@
       </c>
       <c r="D222" s="6" t="inlineStr">
         <is>
-          <t>DATE</t>
+          <t>DATETIME</t>
         </is>
       </c>
       <c r="E222" s="7" t="inlineStr">
@@ -12574,7 +12574,7 @@
       </c>
       <c r="D228" s="9" t="inlineStr">
         <is>
-          <t>DATE</t>
+          <t>DATETIME</t>
         </is>
       </c>
       <c r="E228" s="10" t="inlineStr">
@@ -12736,7 +12736,7 @@
       </c>
       <c r="D234" s="6" t="inlineStr">
         <is>
-          <t>DATE</t>
+          <t>DATETIME</t>
         </is>
       </c>
       <c r="E234" s="7" t="inlineStr">
@@ -12952,7 +12952,7 @@
       </c>
       <c r="D242" s="9" t="inlineStr">
         <is>
-          <t>DATE</t>
+          <t>DATETIME</t>
         </is>
       </c>
       <c r="E242" s="10" t="inlineStr">
@@ -13168,7 +13168,7 @@
       </c>
       <c r="D250" s="6" t="inlineStr">
         <is>
-          <t>DATE</t>
+          <t>DATETIME</t>
         </is>
       </c>
       <c r="E250" s="7" t="inlineStr">
@@ -13411,7 +13411,7 @@
       </c>
       <c r="D259" s="9" t="inlineStr">
         <is>
-          <t>DATE</t>
+          <t>DATETIME</t>
         </is>
       </c>
       <c r="E259" s="10" t="inlineStr">
@@ -13573,7 +13573,7 @@
       </c>
       <c r="D265" s="6" t="inlineStr">
         <is>
-          <t>DATE</t>
+          <t>DATETIME</t>
         </is>
       </c>
       <c r="E265" s="7" t="inlineStr">
@@ -13762,7 +13762,7 @@
       </c>
       <c r="D272" s="9" t="inlineStr">
         <is>
-          <t>DATE</t>
+          <t>DATETIME</t>
         </is>
       </c>
       <c r="E272" s="10" t="inlineStr">
@@ -13951,7 +13951,7 @@
       </c>
       <c r="D279" s="6" t="inlineStr">
         <is>
-          <t>DATE</t>
+          <t>DATETIME</t>
         </is>
       </c>
       <c r="E279" s="7" t="inlineStr">
@@ -14086,7 +14086,7 @@
       </c>
       <c r="D284" s="9" t="inlineStr">
         <is>
-          <t>DATE</t>
+          <t>DATETIME</t>
         </is>
       </c>
       <c r="E284" s="10" t="inlineStr">
@@ -14248,7 +14248,7 @@
       </c>
       <c r="D290" s="6" t="inlineStr">
         <is>
-          <t>DATE</t>
+          <t>DATETIME</t>
         </is>
       </c>
       <c r="E290" s="7" t="inlineStr">
@@ -14437,7 +14437,7 @@
       </c>
       <c r="D297" s="9" t="inlineStr">
         <is>
-          <t>DATE</t>
+          <t>DATETIME</t>
         </is>
       </c>
       <c r="E297" s="10" t="inlineStr">
@@ -14653,7 +14653,7 @@
       </c>
       <c r="D305" s="6" t="inlineStr">
         <is>
-          <t>DATE</t>
+          <t>DATETIME</t>
         </is>
       </c>
       <c r="E305" s="7" t="inlineStr">
@@ -14815,7 +14815,7 @@
       </c>
       <c r="D311" s="9" t="inlineStr">
         <is>
-          <t>DATE</t>
+          <t>DATETIME</t>
         </is>
       </c>
       <c r="E311" s="10" t="inlineStr">
@@ -15004,7 +15004,7 @@
       </c>
       <c r="D318" s="6" t="inlineStr">
         <is>
-          <t>DATE</t>
+          <t>DATETIME</t>
         </is>
       </c>
       <c r="E318" s="7" t="inlineStr">
@@ -15139,7 +15139,7 @@
       </c>
       <c r="D323" s="9" t="inlineStr">
         <is>
-          <t>DATE</t>
+          <t>DATETIME</t>
         </is>
       </c>
       <c r="E323" s="10" t="inlineStr">
@@ -21571,7 +21571,7 @@
       <c r="A2" s="14" t="inlineStr">
         <is>
           <t xml:space="preserve">
-        type: date
+        type: datetime
         </t>
         </is>
       </c>

</xml_diff>